<commit_message>
some issue in js
</commit_message>
<xml_diff>
--- a/Chat1.xlsx
+++ b/Chat1.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anand/Documents/Magic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\MyWorks\Rasa\reservationbot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A4928E-5395-3349-8B84-13137BD2C2F7}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{94DAEEC5-BF4C-DF44-965E-D605CBEB74DD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -194,7 +193,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -573,28 +572,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{706AFA7D-B7BB-F649-9195-C80E7D57C71E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="40.83203125" style="1" customWidth="1"/>
-    <col min="7" max="8" width="10.83203125" style="1"/>
-    <col min="9" max="9" width="25.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="40.875" style="1" customWidth="1"/>
+    <col min="7" max="8" width="10.875" style="1"/>
+    <col min="9" max="9" width="25.375" style="1" customWidth="1"/>
     <col min="10" max="10" width="19" style="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
+    <col min="11" max="11" width="10.875" style="1"/>
     <col min="12" max="12" width="28.5" style="1" customWidth="1"/>
-    <col min="13" max="13" width="47.1640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.83203125" style="1"/>
-    <col min="15" max="15" width="46.1640625" style="1" customWidth="1"/>
-    <col min="16" max="34" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="47.125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.875" style="1"/>
+    <col min="15" max="15" width="46.125" style="1" customWidth="1"/>
+    <col min="16" max="34" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="L2" s="1" t="s">
         <v>48</v>
       </c>
@@ -602,7 +601,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="35" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:17" ht="33.75" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>1</v>
       </c>
@@ -622,7 +621,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -640,7 +639,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>1</v>
       </c>
@@ -657,7 +656,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -674,7 +673,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -694,7 +693,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -708,7 +707,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>1</v>
       </c>
@@ -719,7 +718,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -727,7 +726,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -735,7 +734,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -743,7 +742,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:17" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>1</v>
       </c>
@@ -751,7 +750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:17" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -762,7 +761,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="170" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -773,7 +772,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -781,7 +780,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>1</v>
       </c>
@@ -789,7 +788,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -797,7 +796,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="85" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>1</v>
       </c>
@@ -808,7 +807,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -816,7 +815,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>1</v>
       </c>
@@ -824,7 +823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -832,7 +831,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>1</v>
       </c>
@@ -840,7 +839,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="26" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -848,7 +847,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>1</v>
       </c>
@@ -856,7 +855,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -864,7 +863,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>1</v>
       </c>
@@ -872,7 +871,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -880,7 +879,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:7" ht="34" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>1</v>
       </c>
@@ -888,7 +887,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="32" spans="1:7" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -896,7 +895,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:6" ht="34" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>1</v>
       </c>
@@ -904,102 +903,102 @@
         <v>47</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>1</v>
       </c>

</xml_diff>